<commit_message>
changed run loop, and myopic input creation
</commit_message>
<xml_diff>
--- a/myopic/input/longtable.xlsx
+++ b/myopic/input/longtable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\programming\thesis\urbs\myopic\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB565AD-EFB8-4845-88CA-6F345DE0E3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8947C2-748C-40E1-81AE-FB0C20F3948C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{2550D6F6-3412-4AFF-951F-F0AA6F8F82E1}"/>
   </bookViews>
@@ -700,7 +700,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -769,19 +769,19 @@
         <v>52</v>
       </c>
       <c r="E2" s="10">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="F2" s="10">
         <f>E2*0.5</f>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G2" s="10">
         <f t="shared" ref="G2:H2" si="0">F2*0.5</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H2" s="10">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I2" s="10">
         <v>0</v>
@@ -889,27 +889,21 @@
         <v>2.6</v>
       </c>
       <c r="F5" s="9">
-        <f t="shared" ref="F5:K12" si="1">E5*1.02</f>
         <v>2.6520000000000001</v>
       </c>
       <c r="G5" s="9">
-        <f t="shared" si="1"/>
         <v>2.7050400000000003</v>
       </c>
       <c r="H5" s="9">
-        <f t="shared" si="1"/>
         <v>2.7591408000000004</v>
       </c>
       <c r="I5" s="9">
-        <f t="shared" si="1"/>
         <v>2.8143236160000002</v>
       </c>
       <c r="J5" s="9">
-        <f t="shared" si="1"/>
         <v>2.8706100883200003</v>
       </c>
       <c r="K5" s="9">
-        <f t="shared" si="1"/>
         <v>2.9280222900864006</v>
       </c>
       <c r="L5" s="3" t="s">
@@ -933,27 +927,21 @@
         <v>7</v>
       </c>
       <c r="F6" s="9">
-        <f t="shared" si="1"/>
         <v>7.1400000000000006</v>
       </c>
       <c r="G6" s="9">
-        <f t="shared" si="1"/>
         <v>7.2828000000000008</v>
       </c>
       <c r="H6" s="9">
-        <f t="shared" si="1"/>
         <v>7.4284560000000006</v>
       </c>
       <c r="I6" s="9">
-        <f t="shared" si="1"/>
         <v>7.5770251200000009</v>
       </c>
       <c r="J6" s="9">
-        <f t="shared" si="1"/>
         <v>7.7285656224000014</v>
       </c>
       <c r="K6" s="9">
-        <f t="shared" si="1"/>
         <v>7.883136934848002</v>
       </c>
       <c r="L6" s="3" t="s">
@@ -977,28 +965,22 @@
         <v>8.15</v>
       </c>
       <c r="F7" s="9">
-        <f t="shared" si="1"/>
-        <v>8.3130000000000006</v>
+        <v>27.741091302211302</v>
       </c>
       <c r="G7" s="9">
-        <f t="shared" si="1"/>
-        <v>8.47926</v>
+        <v>47.332182604422606</v>
       </c>
       <c r="H7" s="9">
-        <f t="shared" si="1"/>
-        <v>8.6488452000000002</v>
+        <v>56.805584594594592</v>
       </c>
       <c r="I7" s="9">
-        <f t="shared" si="1"/>
-        <v>8.8218221040000007</v>
+        <v>66.278986584766585</v>
       </c>
       <c r="J7" s="9">
-        <f t="shared" si="1"/>
-        <v>8.9982585460800006</v>
+        <v>72.757548574938568</v>
       </c>
       <c r="K7" s="9">
-        <f t="shared" si="1"/>
-        <v>9.1782237170016003</v>
+        <v>79.236110565110565</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>18</v>
@@ -1021,28 +1003,22 @@
         <v>20.100000000000001</v>
       </c>
       <c r="F8" s="9">
-        <f t="shared" si="1"/>
         <v>20.502000000000002</v>
       </c>
       <c r="G8" s="9">
-        <f t="shared" si="1"/>
-        <v>20.912040000000005</v>
+        <v>27.992005949288941</v>
       </c>
       <c r="H8" s="9">
-        <f t="shared" si="1"/>
-        <v>21.330280800000004</v>
+        <v>31.736446522217683</v>
       </c>
       <c r="I8" s="9">
-        <f t="shared" si="1"/>
-        <v>21.756886416000004</v>
+        <v>35.480887095146429</v>
       </c>
       <c r="J8" s="9">
-        <f t="shared" si="1"/>
-        <v>22.192024144320005</v>
+        <v>37.93953455115517</v>
       </c>
       <c r="K8" s="9">
-        <f t="shared" si="1"/>
-        <v>22.635864627206406</v>
+        <v>40.398182007163911</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>18</v>
@@ -1062,31 +1038,25 @@
         <v>52</v>
       </c>
       <c r="E9" s="11">
-        <v>50</v>
+        <v>50.46240705882353</v>
       </c>
       <c r="F9" s="9">
-        <f t="shared" si="1"/>
-        <v>51</v>
+        <v>50.46240705882353</v>
       </c>
       <c r="G9" s="9">
-        <f t="shared" si="1"/>
-        <v>52.02</v>
+        <v>50.46240705882353</v>
       </c>
       <c r="H9" s="9">
-        <f t="shared" si="1"/>
-        <v>53.060400000000001</v>
+        <v>56.764982647058829</v>
       </c>
       <c r="I9" s="9">
-        <f t="shared" si="1"/>
-        <v>54.121608000000002</v>
+        <v>63.067558235294122</v>
       </c>
       <c r="J9" s="9">
-        <f t="shared" si="1"/>
-        <v>55.204040160000005</v>
+        <v>67.009793823529421</v>
       </c>
       <c r="K9" s="9">
-        <f t="shared" si="1"/>
-        <v>56.308120963200004</v>
+        <v>70.952029411764713</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>18</v>
@@ -1109,27 +1079,21 @@
         <v>55</v>
       </c>
       <c r="F10" s="9">
-        <f t="shared" si="1"/>
         <v>56.1</v>
       </c>
       <c r="G10" s="9">
-        <f t="shared" si="1"/>
         <v>57.222000000000001</v>
       </c>
       <c r="H10" s="9">
-        <f t="shared" si="1"/>
         <v>58.366440000000004</v>
       </c>
       <c r="I10" s="9">
-        <f t="shared" si="1"/>
         <v>59.533768800000004</v>
       </c>
       <c r="J10" s="9">
-        <f t="shared" si="1"/>
         <v>60.724444176000006</v>
       </c>
       <c r="K10" s="9">
-        <f t="shared" si="1"/>
         <v>61.938933059520004</v>
       </c>
       <c r="L10" s="3" t="s">
@@ -1150,31 +1114,25 @@
         <v>52</v>
       </c>
       <c r="E11" s="11">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F11" s="9">
-        <f>E11*1.02</f>
-        <v>10.199999999999999</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="G11" s="9">
-        <f t="shared" si="1"/>
-        <v>10.404</v>
+        <v>20.808</v>
       </c>
       <c r="H11" s="9">
-        <f t="shared" si="1"/>
-        <v>10.612080000000001</v>
+        <v>21.224160000000001</v>
       </c>
       <c r="I11" s="9">
-        <f t="shared" si="1"/>
-        <v>10.824321600000001</v>
+        <v>21.648643200000002</v>
       </c>
       <c r="J11" s="9">
-        <f t="shared" si="1"/>
-        <v>11.040808032000001</v>
+        <v>22.081616064000002</v>
       </c>
       <c r="K11" s="9">
-        <f t="shared" si="1"/>
-        <v>11.261624192640001</v>
+        <v>22.523248385280002</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>18</v>
@@ -1197,28 +1155,22 @@
         <v>100</v>
       </c>
       <c r="F12" s="11">
-        <f>E12*1.02</f>
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G12" s="11">
-        <f t="shared" si="1"/>
-        <v>104.04</v>
+        <v>100</v>
       </c>
       <c r="H12" s="11">
-        <f t="shared" si="1"/>
-        <v>106.1208</v>
+        <v>100</v>
       </c>
       <c r="I12" s="11">
-        <f t="shared" si="1"/>
-        <v>108.243216</v>
+        <v>100</v>
       </c>
       <c r="J12" s="11">
-        <f t="shared" si="1"/>
-        <v>110.40808032000001</v>
+        <v>100</v>
       </c>
       <c r="K12" s="11">
-        <f t="shared" si="1"/>
-        <v>112.61624192640001</v>
+        <v>100</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>18</v>
@@ -2939,27 +2891,27 @@
         <v>3392000</v>
       </c>
       <c r="F57" s="9">
-        <f t="shared" ref="F57:K57" si="2">3392*1000</f>
+        <f t="shared" ref="F57:K57" si="1">3392*1000</f>
         <v>3392000</v>
       </c>
       <c r="G57" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3392000</v>
       </c>
       <c r="H57" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3392000</v>
       </c>
       <c r="I57" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3392000</v>
       </c>
       <c r="J57" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3392000</v>
       </c>
       <c r="K57" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3392000</v>
       </c>
       <c r="L57" s="3" t="s">
@@ -3136,27 +3088,27 @@
         <v>7940450</v>
       </c>
       <c r="F62" s="15">
-        <f t="shared" ref="F62:K62" si="3">MAX(F53:F61)</f>
+        <f t="shared" ref="F62:K62" si="2">MAX(F53:F61)</f>
         <v>7940450</v>
       </c>
       <c r="G62" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7940450</v>
       </c>
       <c r="H62" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7940450</v>
       </c>
       <c r="I62" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7940450</v>
       </c>
       <c r="J62" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7940450</v>
       </c>
       <c r="K62" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7940450</v>
       </c>
       <c r="L62" s="3" t="s">

</xml_diff>